<commit_message>
Test NMSW-552 Handle duplicate person error
</commit_message>
<xml_diff>
--- a/cypress/fixtures/Fal1-Files/General declaration FAL 1-Positive-test.xlsx
+++ b/cypress/fixtures/Fal1-Files/General declaration FAL 1-Positive-test.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Homeoffice\NMSW-VS\nmsw-ui\cypress\fixtures\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Homeoffice\NMSW-Main\nmsw-ui\cypress\fixtures\Fal1-Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CD23871-884A-4F9D-9D91-642FAB3254BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32EF7842-2384-4AB5-8AA0-E7C205607067}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="559">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="560">
   <si>
     <t>UK NMSW FAL 1: General Declaration</t>
   </si>
@@ -2451,6 +2451,9 @@
   </si>
   <si>
     <t>GBXXX</t>
+  </si>
+  <si>
+    <t>C1234</t>
   </si>
 </sst>
 </file>
@@ -4668,8 +4671,8 @@
   </sheetPr>
   <dimension ref="A1:P26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -4722,8 +4725,8 @@
       <c r="E3" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="26">
-        <v>1234</v>
+      <c r="F3" s="26" t="s">
+        <v>559</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="149.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -7209,6 +7212,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="18390984-f7d9-4502-80ba-82ec344db5fb">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="629dd2dc-abea-47e8-ba88-82202e3ee8ef" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D364DC965387FD4EAF4833DDCF640F91" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c7401bc8bddc44f3d87e6545050f3282">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="18390984-f7d9-4502-80ba-82ec344db5fb" xmlns:ns3="629dd2dc-abea-47e8-ba88-82202e3ee8ef" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fc3cb6a02f8baa81433631181c409fee" ns2:_="" ns3:_="">
     <xsd:import namespace="18390984-f7d9-4502-80ba-82ec344db5fb"/>
@@ -7445,27 +7468,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="18390984-f7d9-4502-80ba-82ec344db5fb">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="629dd2dc-abea-47e8-ba88-82202e3ee8ef" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A5056AD-6F82-4433-81E7-2CF7DDF58706}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C2A0AF4-2234-45DE-BCD6-060ACA865D30}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="18390984-f7d9-4502-80ba-82ec344db5fb"/>
+    <ds:schemaRef ds:uri="629dd2dc-abea-47e8-ba88-82202e3ee8ef"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A6CC910-0FFF-41DD-A80E-A1312D067115}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7482,23 +7504,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C2A0AF4-2234-45DE-BCD6-060ACA865D30}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="18390984-f7d9-4502-80ba-82ec344db5fb"/>
-    <ds:schemaRef ds:uri="629dd2dc-abea-47e8-ba88-82202e3ee8ef"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A5056AD-6F82-4433-81E7-2CF7DDF58706}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Change in files data
</commit_message>
<xml_diff>
--- a/cypress/fixtures/Fal1-Files/General declaration FAL 1-Positive-test.xlsx
+++ b/cypress/fixtures/Fal1-Files/General declaration FAL 1-Positive-test.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Homeoffice\NMSW-Main\nmsw-ui\cypress\fixtures\Fal1-Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D5E71AA-AD36-41C1-A114-04457F282D9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{778CC112-DA27-4885-9BB5-4CE0E0ED7BD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2429,31 +2429,31 @@
     </r>
   </si>
   <si>
-    <t>NMSW Test Ship</t>
-  </si>
-  <si>
     <t>Auto Tester</t>
   </si>
   <si>
-    <t>USXXX</t>
-  </si>
-  <si>
     <t>Materials</t>
   </si>
   <si>
     <t>C1234</t>
   </si>
   <si>
-    <t>Departure from the UK</t>
-  </si>
-  <si>
     <t>LKCMB</t>
   </si>
   <si>
-    <t>GBABC</t>
-  </si>
-  <si>
     <t>Hardware and Textiles</t>
+  </si>
+  <si>
+    <t>GBDVR</t>
+  </si>
+  <si>
+    <t>USHNL</t>
+  </si>
+  <si>
+    <t>Arrival in the UK</t>
+  </si>
+  <si>
+    <t>New NMSW Test Ship</t>
   </si>
 </sst>
 </file>
@@ -3373,6 +3373,7 @@
     <xf numFmtId="14" fontId="20" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="14" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3481,7 +3482,6 @@
     <xf numFmtId="49" fontId="0" fillId="8" borderId="34" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4678,8 +4678,8 @@
   </sheetPr>
   <dimension ref="A1:P26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10:D26"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -4695,33 +4695,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
     </row>
     <row r="2" spans="1:6" ht="102" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="31" t="s">
-        <v>556</v>
-      </c>
-      <c r="C2" s="51"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="53"/>
+        <v>558</v>
+      </c>
+      <c r="C2" s="52"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="54"/>
     </row>
     <row r="3" spans="1:6" ht="90.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="40" t="s">
-        <v>551</v>
+        <v>559</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>3</v>
@@ -4733,7 +4733,7 @@
         <v>4</v>
       </c>
       <c r="F3" s="26" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="149.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -4741,7 +4741,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="40" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>6</v>
@@ -4749,15 +4749,15 @@
       <c r="D4" s="40" t="s">
         <v>118</v>
       </c>
-      <c r="E4" s="58"/>
-      <c r="F4" s="59"/>
+      <c r="E4" s="59"/>
+      <c r="F4" s="60"/>
     </row>
     <row r="5" spans="1:6" ht="270" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="40" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>8</v>
@@ -4777,7 +4777,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="40" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>11</v>
@@ -4803,13 +4803,13 @@
         <v>14</v>
       </c>
       <c r="D7" s="41" t="s">
-        <v>553</v>
+        <v>557</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>15</v>
       </c>
       <c r="F7" s="42" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4825,15 +4825,15 @@
       <c r="D8" s="38">
         <v>10</v>
       </c>
-      <c r="E8" s="54"/>
-      <c r="F8" s="54"/>
+      <c r="E8" s="55"/>
+      <c r="F8" s="55"/>
     </row>
     <row r="9" spans="1:6" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B9" s="43" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>19</v>
@@ -4841,8 +4841,8 @@
       <c r="D9" s="34">
         <v>987654321</v>
       </c>
-      <c r="E9" s="55"/>
-      <c r="F9" s="54"/>
+      <c r="E9" s="56"/>
+      <c r="F9" s="55"/>
     </row>
     <row r="10" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="10" t="s">
@@ -4851,10 +4851,10 @@
       <c r="B10" s="44" t="s">
         <v>118</v>
       </c>
-      <c r="C10" s="60"/>
-      <c r="D10" s="61"/>
-      <c r="E10" s="55"/>
-      <c r="F10" s="54"/>
+      <c r="C10" s="61"/>
+      <c r="D10" s="62"/>
+      <c r="E10" s="56"/>
+      <c r="F10" s="55"/>
     </row>
     <row r="11" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="10" t="s">
@@ -4863,34 +4863,34 @@
       <c r="B11" s="34">
         <v>5</v>
       </c>
-      <c r="C11" s="62"/>
-      <c r="D11" s="63"/>
-      <c r="E11" s="55"/>
-      <c r="F11" s="54"/>
+      <c r="C11" s="63"/>
+      <c r="D11" s="64"/>
+      <c r="E11" s="56"/>
+      <c r="F11" s="55"/>
     </row>
     <row r="12" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="10" t="s">
         <v>22</v>
       </c>
       <c r="B12" s="45" t="s">
-        <v>554</v>
-      </c>
-      <c r="C12" s="62"/>
-      <c r="D12" s="63"/>
-      <c r="E12" s="55"/>
-      <c r="F12" s="54"/>
+        <v>552</v>
+      </c>
+      <c r="C12" s="63"/>
+      <c r="D12" s="64"/>
+      <c r="E12" s="56"/>
+      <c r="F12" s="55"/>
     </row>
     <row r="13" spans="1:6" ht="128.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="84" t="s">
-        <v>559</v>
-      </c>
-      <c r="C13" s="62"/>
-      <c r="D13" s="63"/>
-      <c r="E13" s="55"/>
-      <c r="F13" s="54"/>
+      <c r="B13" s="48" t="s">
+        <v>555</v>
+      </c>
+      <c r="C13" s="63"/>
+      <c r="D13" s="64"/>
+      <c r="E13" s="56"/>
+      <c r="F13" s="55"/>
     </row>
     <row r="14" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="12" t="s">
@@ -4899,10 +4899,10 @@
       <c r="B14" s="35">
         <v>20</v>
       </c>
-      <c r="C14" s="62"/>
-      <c r="D14" s="63"/>
-      <c r="E14" s="55"/>
-      <c r="F14" s="54"/>
+      <c r="C14" s="63"/>
+      <c r="D14" s="64"/>
+      <c r="E14" s="56"/>
+      <c r="F14" s="55"/>
     </row>
     <row r="15" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="7" t="s">
@@ -4911,120 +4911,120 @@
       <c r="B15" s="36">
         <v>100</v>
       </c>
-      <c r="C15" s="62"/>
-      <c r="D15" s="63"/>
-      <c r="E15" s="55"/>
-      <c r="F15" s="54"/>
+      <c r="C15" s="63"/>
+      <c r="D15" s="64"/>
+      <c r="E15" s="56"/>
+      <c r="F15" s="55"/>
     </row>
     <row r="16" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="7" t="s">
         <v>26</v>
       </c>
       <c r="B16" s="33"/>
-      <c r="C16" s="62"/>
-      <c r="D16" s="63"/>
-      <c r="E16" s="55"/>
-      <c r="F16" s="54"/>
+      <c r="C16" s="63"/>
+      <c r="D16" s="64"/>
+      <c r="E16" s="56"/>
+      <c r="F16" s="55"/>
     </row>
     <row r="17" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="56" t="s">
+      <c r="A17" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="57"/>
-      <c r="C17" s="62"/>
-      <c r="D17" s="63"/>
-      <c r="E17" s="55"/>
-      <c r="F17" s="54"/>
+      <c r="B17" s="58"/>
+      <c r="C17" s="63"/>
+      <c r="D17" s="64"/>
+      <c r="E17" s="56"/>
+      <c r="F17" s="55"/>
     </row>
     <row r="18" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A18" s="7" t="s">
         <v>28</v>
       </c>
       <c r="B18" s="27"/>
-      <c r="C18" s="62"/>
-      <c r="D18" s="63"/>
-      <c r="E18" s="55"/>
-      <c r="F18" s="54"/>
+      <c r="C18" s="63"/>
+      <c r="D18" s="64"/>
+      <c r="E18" s="56"/>
+      <c r="F18" s="55"/>
     </row>
     <row r="19" spans="1:6" ht="33" x14ac:dyDescent="0.35">
       <c r="A19" s="7" t="s">
         <v>29</v>
       </c>
       <c r="B19" s="27"/>
-      <c r="C19" s="62"/>
-      <c r="D19" s="63"/>
-      <c r="E19" s="55"/>
-      <c r="F19" s="54"/>
+      <c r="C19" s="63"/>
+      <c r="D19" s="64"/>
+      <c r="E19" s="56"/>
+      <c r="F19" s="55"/>
     </row>
     <row r="20" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
         <v>30</v>
       </c>
       <c r="B20" s="27"/>
-      <c r="C20" s="62"/>
-      <c r="D20" s="63"/>
-      <c r="E20" s="55"/>
-      <c r="F20" s="54"/>
+      <c r="C20" s="63"/>
+      <c r="D20" s="64"/>
+      <c r="E20" s="56"/>
+      <c r="F20" s="55"/>
     </row>
     <row r="21" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="7" t="s">
         <v>31</v>
       </c>
       <c r="B21" s="27"/>
-      <c r="C21" s="62"/>
-      <c r="D21" s="63"/>
-      <c r="E21" s="55"/>
-      <c r="F21" s="54"/>
+      <c r="C21" s="63"/>
+      <c r="D21" s="64"/>
+      <c r="E21" s="56"/>
+      <c r="F21" s="55"/>
     </row>
     <row r="22" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B22" s="27"/>
-      <c r="C22" s="62"/>
-      <c r="D22" s="63"/>
-      <c r="E22" s="55"/>
-      <c r="F22" s="54"/>
+      <c r="C22" s="63"/>
+      <c r="D22" s="64"/>
+      <c r="E22" s="56"/>
+      <c r="F22" s="55"/>
     </row>
     <row r="23" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="7" t="s">
         <v>33</v>
       </c>
       <c r="B23" s="27"/>
-      <c r="C23" s="62"/>
-      <c r="D23" s="63"/>
-      <c r="E23" s="55"/>
-      <c r="F23" s="54"/>
+      <c r="C23" s="63"/>
+      <c r="D23" s="64"/>
+      <c r="E23" s="56"/>
+      <c r="F23" s="55"/>
     </row>
     <row r="24" spans="1:6" ht="17.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="7" t="s">
         <v>34</v>
       </c>
       <c r="B24" s="27"/>
-      <c r="C24" s="62"/>
-      <c r="D24" s="63"/>
-      <c r="E24" s="55"/>
-      <c r="F24" s="54"/>
+      <c r="C24" s="63"/>
+      <c r="D24" s="64"/>
+      <c r="E24" s="56"/>
+      <c r="F24" s="55"/>
     </row>
     <row r="25" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="7" t="s">
         <v>35</v>
       </c>
       <c r="B25" s="37"/>
-      <c r="C25" s="62"/>
-      <c r="D25" s="63"/>
-      <c r="E25" s="55"/>
-      <c r="F25" s="54"/>
+      <c r="C25" s="63"/>
+      <c r="D25" s="64"/>
+      <c r="E25" s="56"/>
+      <c r="F25" s="55"/>
     </row>
     <row r="26" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="11" t="s">
         <v>36</v>
       </c>
       <c r="B26" s="27"/>
-      <c r="C26" s="64"/>
-      <c r="D26" s="65"/>
-      <c r="E26" s="55"/>
-      <c r="F26" s="54"/>
+      <c r="C26" s="65"/>
+      <c r="D26" s="66"/>
+      <c r="E26" s="56"/>
+      <c r="F26" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -5083,11 +5083,11 @@
       <c r="B1" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="69" t="s">
+      <c r="C1" s="70" t="s">
         <v>39</v>
       </c>
-      <c r="D1" s="70"/>
-      <c r="E1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="72"/>
       <c r="F1" s="19"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -5097,9 +5097,9 @@
       <c r="B2" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="72"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="74"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="75"/>
       <c r="F2" s="19"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -5109,11 +5109,11 @@
       <c r="B3" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="66" t="s">
+      <c r="C3" s="67" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="67"/>
-      <c r="E3" s="68"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="69"/>
       <c r="F3" s="19"/>
     </row>
     <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -5123,11 +5123,11 @@
       <c r="B4" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="C4" s="75" t="s">
+      <c r="C4" s="76" t="s">
         <v>47</v>
       </c>
-      <c r="D4" s="76"/>
-      <c r="E4" s="77"/>
+      <c r="D4" s="77"/>
+      <c r="E4" s="78"/>
       <c r="F4" s="19"/>
     </row>
     <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -5137,9 +5137,9 @@
       <c r="B5" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="C5" s="78"/>
-      <c r="D5" s="79"/>
-      <c r="E5" s="80"/>
+      <c r="C5" s="79"/>
+      <c r="D5" s="80"/>
+      <c r="E5" s="81"/>
       <c r="F5" s="19"/>
     </row>
     <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -5149,9 +5149,9 @@
       <c r="B6" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="C6" s="81"/>
-      <c r="D6" s="82"/>
-      <c r="E6" s="83"/>
+      <c r="C6" s="82"/>
+      <c r="D6" s="83"/>
+      <c r="E6" s="84"/>
       <c r="F6" s="19"/>
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -7219,26 +7219,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="18390984-f7d9-4502-80ba-82ec344db5fb">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="629dd2dc-abea-47e8-ba88-82202e3ee8ef" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D364DC965387FD4EAF4833DDCF640F91" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c7401bc8bddc44f3d87e6545050f3282">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="18390984-f7d9-4502-80ba-82ec344db5fb" xmlns:ns3="629dd2dc-abea-47e8-ba88-82202e3ee8ef" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fc3cb6a02f8baa81433631181c409fee" ns2:_="" ns3:_="">
     <xsd:import namespace="18390984-f7d9-4502-80ba-82ec344db5fb"/>
@@ -7475,26 +7455,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C2A0AF4-2234-45DE-BCD6-060ACA865D30}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="18390984-f7d9-4502-80ba-82ec344db5fb"/>
-    <ds:schemaRef ds:uri="629dd2dc-abea-47e8-ba88-82202e3ee8ef"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="18390984-f7d9-4502-80ba-82ec344db5fb">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="629dd2dc-abea-47e8-ba88-82202e3ee8ef" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A5056AD-6F82-4433-81E7-2CF7DDF58706}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A6CC910-0FFF-41DD-A80E-A1312D067115}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7511,4 +7492,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C2A0AF4-2234-45DE-BCD6-060ACA865D30}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="18390984-f7d9-4502-80ba-82ec344db5fb"/>
+    <ds:schemaRef ds:uri="629dd2dc-abea-47e8-ba88-82202e3ee8ef"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A5056AD-6F82-4433-81E7-2CF7DDF58706}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Test accepting spl characters for FAL 5 and 6
</commit_message>
<xml_diff>
--- a/cypress/fixtures/Fal1-Files/General declaration FAL 1-Positive-test.xlsx
+++ b/cypress/fixtures/Fal1-Files/General declaration FAL 1-Positive-test.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Homeoffice\NMSW-Main\nmsw-ui\cypress\fixtures\Fal1-Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Homeoffice\NMSW\nmsw-ui\cypress\fixtures\Fal1-Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{778CC112-DA27-4885-9BB5-4CE0E0ED7BD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95E1F4F1-4EA5-4AC8-B988-269C584B2922}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4678,8 +4678,8 @@
   </sheetPr>
   <dimension ref="A1:P26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -7219,6 +7219,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="18390984-f7d9-4502-80ba-82ec344db5fb">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="629dd2dc-abea-47e8-ba88-82202e3ee8ef" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D364DC965387FD4EAF4833DDCF640F91" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c7401bc8bddc44f3d87e6545050f3282">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="18390984-f7d9-4502-80ba-82ec344db5fb" xmlns:ns3="629dd2dc-abea-47e8-ba88-82202e3ee8ef" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fc3cb6a02f8baa81433631181c409fee" ns2:_="" ns3:_="">
     <xsd:import namespace="18390984-f7d9-4502-80ba-82ec344db5fb"/>
@@ -7455,27 +7475,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="18390984-f7d9-4502-80ba-82ec344db5fb">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="629dd2dc-abea-47e8-ba88-82202e3ee8ef" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C2A0AF4-2234-45DE-BCD6-060ACA865D30}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="18390984-f7d9-4502-80ba-82ec344db5fb"/>
+    <ds:schemaRef ds:uri="629dd2dc-abea-47e8-ba88-82202e3ee8ef"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A5056AD-6F82-4433-81E7-2CF7DDF58706}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A6CC910-0FFF-41DD-A80E-A1312D067115}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7492,23 +7511,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C2A0AF4-2234-45DE-BCD6-060ACA865D30}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="18390984-f7d9-4502-80ba-82ec344db5fb"/>
-    <ds:schemaRef ds:uri="629dd2dc-abea-47e8-ba88-82202e3ee8ef"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A5056AD-6F82-4433-81E7-2CF7DDF58706}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Test to verify CBP accepts  FAL1, FAL5, and FAL6 with carriage return
</commit_message>
<xml_diff>
--- a/cypress/fixtures/Fal1-Files/General declaration FAL 1-Positive-test.xlsx
+++ b/cypress/fixtures/Fal1-Files/General declaration FAL 1-Positive-test.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Homeoffice\NMSWTemp\nmsw-ui\cypress\fixtures\Fal1-Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EC53377-77DB-4A23-BD43-CF9236C0471C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCF574C0-44CB-4F89-BCB9-70B134FA2E97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="560">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="572">
   <si>
     <t>UK NMSW FAL 1: General Declaration</t>
   </si>
@@ -2429,31 +2429,114 @@
     </r>
   </si>
   <si>
-    <t>Auto Tester</t>
-  </si>
-  <si>
-    <t>Materials</t>
-  </si>
-  <si>
-    <t>C1234</t>
-  </si>
-  <si>
     <t>LKCMB</t>
   </si>
   <si>
-    <t>Hardware and Textiles</t>
-  </si>
-  <si>
-    <t>GBDVR</t>
-  </si>
-  <si>
-    <t>USHNL</t>
-  </si>
-  <si>
     <t>Arrival in the UK</t>
   </si>
   <si>
-    <t>New NMSW Test Ship</t>
+    <t>New NMSW Test
+ Ship</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Auto
+ Tester</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+GB
+DVR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+US
+HNL
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Auto
+ Tester
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Auto
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 
+Tester
+Tester
+Tester
+Tester
+Tester
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 
+Test Materials
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Hardware
+ and 
+Textiles
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+20
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+100
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Permitted 
+to
+ carry
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+9999990
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+CAN
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+15/10/2023
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+03/05/2023
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+10
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+987654321
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+C1234
+</t>
   </si>
 </sst>
 </file>
@@ -3232,7 +3315,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3307,9 +3390,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3331,30 +3411,15 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3364,16 +3429,12 @@
     <xf numFmtId="0" fontId="20" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="20" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="14" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3481,6 +3542,24 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="8" borderId="34" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4678,8 +4757,8 @@
   </sheetPr>
   <dimension ref="A1:P26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -4695,80 +4774,80 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
     </row>
     <row r="2" spans="1:6" ht="102" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="31" t="s">
-        <v>558</v>
-      </c>
-      <c r="C2" s="52"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="54"/>
+      <c r="B2" s="30" t="s">
+        <v>552</v>
+      </c>
+      <c r="C2" s="44"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="46"/>
     </row>
     <row r="3" spans="1:6" ht="90.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="40" t="s">
-        <v>559</v>
+      <c r="B3" s="35" t="s">
+        <v>553</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="32">
-        <v>9999990</v>
+      <c r="D3" s="31" t="s">
+        <v>565</v>
       </c>
       <c r="E3" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="26" t="s">
-        <v>553</v>
+      <c r="F3" s="82" t="s">
+        <v>571</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="149.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="40" t="s">
-        <v>551</v>
+      <c r="B4" s="35" t="s">
+        <v>554</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="40" t="s">
-        <v>118</v>
-      </c>
-      <c r="E4" s="59"/>
-      <c r="F4" s="60"/>
+      <c r="D4" s="35" t="s">
+        <v>566</v>
+      </c>
+      <c r="E4" s="51"/>
+      <c r="F4" s="52"/>
     </row>
     <row r="5" spans="1:6" ht="270" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="40" t="s">
-        <v>556</v>
+      <c r="B5" s="35" t="s">
+        <v>555</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="46">
-        <v>45214</v>
+      <c r="D5" s="39" t="s">
+        <v>567</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="39">
+      <c r="F5" s="34">
         <v>0.5</v>
       </c>
     </row>
@@ -4776,19 +4855,19 @@
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="40" t="s">
-        <v>557</v>
+      <c r="B6" s="35" t="s">
+        <v>556</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="47">
-        <v>45049</v>
+      <c r="D6" s="40" t="s">
+        <v>568</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="39">
+      <c r="F6" s="34">
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
@@ -4796,235 +4875,237 @@
       <c r="A7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="30">
+      <c r="B7" s="29">
         <v>100</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="41" t="s">
-        <v>557</v>
+      <c r="D7" s="35" t="s">
+        <v>556</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="42" t="s">
-        <v>554</v>
+      <c r="F7" s="36" t="s">
+        <v>551</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="30">
-        <v>10</v>
+      <c r="B8" s="29">
+        <v>100</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="38">
-        <v>10</v>
-      </c>
-      <c r="E8" s="55"/>
-      <c r="F8" s="55"/>
+      <c r="D8" s="81" t="s">
+        <v>569</v>
+      </c>
+      <c r="E8" s="47"/>
+      <c r="F8" s="47"/>
     </row>
     <row r="9" spans="1:6" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="43" t="s">
-        <v>551</v>
+      <c r="B9" s="37" t="s">
+        <v>557</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="34">
-        <v>987654321</v>
-      </c>
-      <c r="E9" s="56"/>
-      <c r="F9" s="55"/>
+      <c r="D9" s="32" t="s">
+        <v>570</v>
+      </c>
+      <c r="E9" s="48"/>
+      <c r="F9" s="47"/>
     </row>
     <row r="10" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="44" t="s">
-        <v>118</v>
-      </c>
-      <c r="C10" s="61"/>
-      <c r="D10" s="62"/>
-      <c r="E10" s="56"/>
-      <c r="F10" s="55"/>
+      <c r="B10" s="38" t="s">
+        <v>558</v>
+      </c>
+      <c r="C10" s="53"/>
+      <c r="D10" s="54"/>
+      <c r="E10" s="48"/>
+      <c r="F10" s="47"/>
     </row>
     <row r="11" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="34">
-        <v>5</v>
-      </c>
-      <c r="C11" s="63"/>
-      <c r="D11" s="64"/>
-      <c r="E11" s="56"/>
-      <c r="F11" s="55"/>
+      <c r="B11" s="32" t="s">
+        <v>559</v>
+      </c>
+      <c r="C11" s="55"/>
+      <c r="D11" s="56"/>
+      <c r="E11" s="48"/>
+      <c r="F11" s="47"/>
     </row>
     <row r="12" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="45" t="s">
-        <v>552</v>
-      </c>
-      <c r="C12" s="63"/>
-      <c r="D12" s="64"/>
-      <c r="E12" s="56"/>
-      <c r="F12" s="55"/>
+      <c r="B12" s="77" t="s">
+        <v>560</v>
+      </c>
+      <c r="C12" s="55"/>
+      <c r="D12" s="56"/>
+      <c r="E12" s="48"/>
+      <c r="F12" s="47"/>
     </row>
     <row r="13" spans="1:6" ht="128.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="48" t="s">
-        <v>555</v>
-      </c>
-      <c r="C13" s="63"/>
-      <c r="D13" s="64"/>
-      <c r="E13" s="56"/>
-      <c r="F13" s="55"/>
+      <c r="B13" s="78" t="s">
+        <v>561</v>
+      </c>
+      <c r="C13" s="55"/>
+      <c r="D13" s="56"/>
+      <c r="E13" s="48"/>
+      <c r="F13" s="47"/>
     </row>
     <row r="14" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="35">
-        <v>20</v>
-      </c>
-      <c r="C14" s="63"/>
-      <c r="D14" s="64"/>
-      <c r="E14" s="56"/>
-      <c r="F14" s="55"/>
+      <c r="B14" s="79" t="s">
+        <v>562</v>
+      </c>
+      <c r="C14" s="55"/>
+      <c r="D14" s="56"/>
+      <c r="E14" s="48"/>
+      <c r="F14" s="47"/>
     </row>
     <row r="15" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="36">
-        <v>100</v>
-      </c>
-      <c r="C15" s="63"/>
-      <c r="D15" s="64"/>
-      <c r="E15" s="56"/>
-      <c r="F15" s="55"/>
+      <c r="B15" s="80" t="s">
+        <v>563</v>
+      </c>
+      <c r="C15" s="55"/>
+      <c r="D15" s="56"/>
+      <c r="E15" s="48"/>
+      <c r="F15" s="47"/>
     </row>
     <row r="16" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="33"/>
-      <c r="C16" s="63"/>
-      <c r="D16" s="64"/>
-      <c r="E16" s="56"/>
-      <c r="F16" s="55"/>
+      <c r="B16" s="32" t="s">
+        <v>564</v>
+      </c>
+      <c r="C16" s="55"/>
+      <c r="D16" s="56"/>
+      <c r="E16" s="48"/>
+      <c r="F16" s="47"/>
     </row>
     <row r="17" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="57" t="s">
+      <c r="A17" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="58"/>
-      <c r="C17" s="63"/>
-      <c r="D17" s="64"/>
-      <c r="E17" s="56"/>
-      <c r="F17" s="55"/>
+      <c r="B17" s="50"/>
+      <c r="C17" s="55"/>
+      <c r="D17" s="56"/>
+      <c r="E17" s="48"/>
+      <c r="F17" s="47"/>
     </row>
     <row r="18" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A18" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B18" s="27"/>
-      <c r="C18" s="63"/>
-      <c r="D18" s="64"/>
-      <c r="E18" s="56"/>
-      <c r="F18" s="55"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="55"/>
+      <c r="D18" s="56"/>
+      <c r="E18" s="48"/>
+      <c r="F18" s="47"/>
     </row>
     <row r="19" spans="1:6" ht="33" x14ac:dyDescent="0.35">
       <c r="A19" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="27"/>
-      <c r="C19" s="63"/>
-      <c r="D19" s="64"/>
-      <c r="E19" s="56"/>
-      <c r="F19" s="55"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="55"/>
+      <c r="D19" s="56"/>
+      <c r="E19" s="48"/>
+      <c r="F19" s="47"/>
     </row>
     <row r="20" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B20" s="27"/>
-      <c r="C20" s="63"/>
-      <c r="D20" s="64"/>
-      <c r="E20" s="56"/>
-      <c r="F20" s="55"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="55"/>
+      <c r="D20" s="56"/>
+      <c r="E20" s="48"/>
+      <c r="F20" s="47"/>
     </row>
     <row r="21" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="27"/>
-      <c r="C21" s="63"/>
-      <c r="D21" s="64"/>
-      <c r="E21" s="56"/>
-      <c r="F21" s="55"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="55"/>
+      <c r="D21" s="56"/>
+      <c r="E21" s="48"/>
+      <c r="F21" s="47"/>
     </row>
     <row r="22" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B22" s="27"/>
-      <c r="C22" s="63"/>
-      <c r="D22" s="64"/>
-      <c r="E22" s="56"/>
-      <c r="F22" s="55"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="55"/>
+      <c r="D22" s="56"/>
+      <c r="E22" s="48"/>
+      <c r="F22" s="47"/>
     </row>
     <row r="23" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B23" s="27"/>
-      <c r="C23" s="63"/>
-      <c r="D23" s="64"/>
-      <c r="E23" s="56"/>
-      <c r="F23" s="55"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="55"/>
+      <c r="D23" s="56"/>
+      <c r="E23" s="48"/>
+      <c r="F23" s="47"/>
     </row>
     <row r="24" spans="1:6" ht="17.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B24" s="27"/>
-      <c r="C24" s="63"/>
-      <c r="D24" s="64"/>
-      <c r="E24" s="56"/>
-      <c r="F24" s="55"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="55"/>
+      <c r="D24" s="56"/>
+      <c r="E24" s="48"/>
+      <c r="F24" s="47"/>
     </row>
     <row r="25" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B25" s="37"/>
-      <c r="C25" s="63"/>
-      <c r="D25" s="64"/>
-      <c r="E25" s="56"/>
-      <c r="F25" s="55"/>
+      <c r="B25" s="33"/>
+      <c r="C25" s="55"/>
+      <c r="D25" s="56"/>
+      <c r="E25" s="48"/>
+      <c r="F25" s="47"/>
     </row>
     <row r="26" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B26" s="27"/>
-      <c r="C26" s="65"/>
-      <c r="D26" s="66"/>
-      <c r="E26" s="56"/>
-      <c r="F26" s="55"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="57"/>
+      <c r="D26" s="58"/>
+      <c r="E26" s="48"/>
+      <c r="F26" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -5070,95 +5151,95 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15.5" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.53515625" style="29" customWidth="1"/>
-    <col min="2" max="2" width="46.84375" style="29" customWidth="1"/>
+    <col min="1" max="1" width="12.53515625" style="28" customWidth="1"/>
+    <col min="2" max="2" width="46.84375" style="28" customWidth="1"/>
     <col min="3" max="5" width="12.53515625" style="16" customWidth="1"/>
     <col min="6" max="16384" width="11.53515625" style="16"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="70" t="s">
+      <c r="C1" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="D1" s="71"/>
-      <c r="E1" s="72"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="64"/>
       <c r="F1" s="19"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="73"/>
-      <c r="D2" s="74"/>
-      <c r="E2" s="75"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="67"/>
       <c r="F2" s="19"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="67" t="s">
+      <c r="C3" s="59" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="68"/>
-      <c r="E3" s="69"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="61"/>
       <c r="F3" s="19"/>
     </row>
     <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="C4" s="76" t="s">
+      <c r="C4" s="68" t="s">
         <v>47</v>
       </c>
-      <c r="D4" s="77"/>
-      <c r="E4" s="78"/>
+      <c r="D4" s="69"/>
+      <c r="E4" s="70"/>
       <c r="F4" s="19"/>
     </row>
     <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="C5" s="79"/>
-      <c r="D5" s="80"/>
-      <c r="E5" s="81"/>
+      <c r="C5" s="71"/>
+      <c r="D5" s="72"/>
+      <c r="E5" s="73"/>
       <c r="F5" s="19"/>
     </row>
     <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="B6" s="28" t="s">
+      <c r="B6" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="C6" s="82"/>
-      <c r="D6" s="83"/>
-      <c r="E6" s="84"/>
+      <c r="C6" s="74"/>
+      <c r="D6" s="75"/>
+      <c r="E6" s="76"/>
       <c r="F6" s="19"/>
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="B7" s="28" t="s">
+      <c r="B7" s="27" t="s">
         <v>53</v>
       </c>
       <c r="C7" s="20"/>
@@ -5166,10 +5247,10 @@
       <c r="E7" s="20"/>
     </row>
     <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="27" t="s">
         <v>55</v>
       </c>
       <c r="C8" s="14"/>
@@ -5177,10 +5258,10 @@
       <c r="E8" s="14"/>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="28" t="s">
+      <c r="A9" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="B9" s="28" t="s">
+      <c r="B9" s="27" t="s">
         <v>57</v>
       </c>
       <c r="C9" s="14"/>
@@ -5188,10 +5269,10 @@
       <c r="E9" s="15"/>
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="28" t="s">
+      <c r="A10" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="B10" s="28" t="s">
+      <c r="B10" s="27" t="s">
         <v>59</v>
       </c>
       <c r="C10" s="14"/>
@@ -5199,10 +5280,10 @@
       <c r="E10" s="15"/>
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="28" t="s">
+      <c r="A11" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="27" t="s">
         <v>61</v>
       </c>
       <c r="C11" s="14"/>
@@ -5210,10 +5291,10 @@
       <c r="E11" s="18"/>
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="28" t="s">
+      <c r="A12" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="B12" s="28" t="s">
+      <c r="B12" s="27" t="s">
         <v>63</v>
       </c>
       <c r="C12" s="14"/>
@@ -5221,1938 +5302,1938 @@
       <c r="E12" s="17"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="28" t="s">
+      <c r="A13" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="B13" s="28" t="s">
+      <c r="B13" s="27" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="28" t="s">
+      <c r="A14" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="B14" s="28" t="s">
+      <c r="B14" s="27" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="28" t="s">
+      <c r="A15" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="B15" s="28" t="s">
+      <c r="B15" s="27" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="28" t="s">
+      <c r="A16" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="B16" s="28" t="s">
+      <c r="B16" s="27" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="28" t="s">
+      <c r="A17" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="B17" s="28" t="s">
+      <c r="B17" s="27" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="28" t="s">
+      <c r="A18" s="27" t="s">
         <v>74</v>
       </c>
-      <c r="B18" s="28" t="s">
+      <c r="B18" s="27" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="28" t="s">
+      <c r="A19" s="27" t="s">
         <v>76</v>
       </c>
-      <c r="B19" s="28" t="s">
+      <c r="B19" s="27" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="28" t="s">
+      <c r="A20" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="B20" s="28" t="s">
+      <c r="B20" s="27" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A21" s="28" t="s">
+      <c r="A21" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="B21" s="28" t="s">
+      <c r="B21" s="27" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="28" t="s">
+      <c r="A22" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="B22" s="28" t="s">
+      <c r="B22" s="27" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="28" t="s">
+      <c r="A23" s="27" t="s">
         <v>84</v>
       </c>
-      <c r="B23" s="28" t="s">
+      <c r="B23" s="27" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="28" t="s">
+      <c r="A24" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="B24" s="28" t="s">
+      <c r="B24" s="27" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="28" t="s">
+      <c r="A25" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="B25" s="28" t="s">
+      <c r="B25" s="27" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="28" t="s">
+      <c r="A26" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="B26" s="28" t="s">
+      <c r="B26" s="27" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="28" t="s">
+      <c r="A27" s="27" t="s">
         <v>92</v>
       </c>
-      <c r="B27" s="28" t="s">
+      <c r="B27" s="27" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="28" t="s">
+      <c r="A28" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="B28" s="28" t="s">
+      <c r="B28" s="27" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="28" t="s">
+      <c r="A29" s="27" t="s">
         <v>96</v>
       </c>
-      <c r="B29" s="28" t="s">
+      <c r="B29" s="27" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="28" t="s">
+      <c r="A30" s="27" t="s">
         <v>98</v>
       </c>
-      <c r="B30" s="28" t="s">
+      <c r="B30" s="27" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="28" t="s">
+      <c r="A31" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="B31" s="28" t="s">
+      <c r="B31" s="27" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="28" t="s">
+      <c r="A32" s="27" t="s">
         <v>102</v>
       </c>
-      <c r="B32" s="28" t="s">
+      <c r="B32" s="27" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="28" t="s">
+      <c r="A33" s="27" t="s">
         <v>104</v>
       </c>
-      <c r="B33" s="28" t="s">
+      <c r="B33" s="27" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="28" t="s">
+      <c r="A34" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="B34" s="28" t="s">
+      <c r="B34" s="27" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="28" t="s">
+      <c r="A35" s="27" t="s">
         <v>108</v>
       </c>
-      <c r="B35" s="28" t="s">
+      <c r="B35" s="27" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="28" t="s">
+      <c r="A36" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="B36" s="28" t="s">
+      <c r="B36" s="27" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="28" t="s">
+      <c r="A37" s="27" t="s">
         <v>112</v>
       </c>
-      <c r="B37" s="28" t="s">
+      <c r="B37" s="27" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="28" t="s">
+      <c r="A38" s="27" t="s">
         <v>114</v>
       </c>
-      <c r="B38" s="28" t="s">
+      <c r="B38" s="27" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="28" t="s">
+      <c r="A39" s="27" t="s">
         <v>116</v>
       </c>
-      <c r="B39" s="28" t="s">
+      <c r="B39" s="27" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="28" t="s">
+      <c r="A40" s="27" t="s">
         <v>118</v>
       </c>
-      <c r="B40" s="28" t="s">
+      <c r="B40" s="27" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="28" t="s">
+      <c r="A41" s="27" t="s">
         <v>120</v>
       </c>
-      <c r="B41" s="28" t="s">
+      <c r="B41" s="27" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="28" t="s">
+      <c r="A42" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="B42" s="28" t="s">
+      <c r="B42" s="27" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="28" t="s">
+      <c r="A43" s="27" t="s">
         <v>124</v>
       </c>
-      <c r="B43" s="28" t="s">
+      <c r="B43" s="27" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="28" t="s">
+      <c r="A44" s="27" t="s">
         <v>126</v>
       </c>
-      <c r="B44" s="28" t="s">
+      <c r="B44" s="27" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="28" t="s">
+      <c r="A45" s="27" t="s">
         <v>128</v>
       </c>
-      <c r="B45" s="28" t="s">
+      <c r="B45" s="27" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="28" t="s">
+      <c r="A46" s="27" t="s">
         <v>130</v>
       </c>
-      <c r="B46" s="28" t="s">
+      <c r="B46" s="27" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="28" t="s">
+      <c r="A47" s="27" t="s">
         <v>132</v>
       </c>
-      <c r="B47" s="28" t="s">
+      <c r="B47" s="27" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="28" t="s">
+      <c r="A48" s="27" t="s">
         <v>134</v>
       </c>
-      <c r="B48" s="28" t="s">
+      <c r="B48" s="27" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="28" t="s">
+      <c r="A49" s="27" t="s">
         <v>136</v>
       </c>
-      <c r="B49" s="28" t="s">
+      <c r="B49" s="27" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="28" t="s">
+      <c r="A50" s="27" t="s">
         <v>138</v>
       </c>
-      <c r="B50" s="28" t="s">
+      <c r="B50" s="27" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="28" t="s">
+      <c r="A51" s="27" t="s">
         <v>140</v>
       </c>
-      <c r="B51" s="28" t="s">
+      <c r="B51" s="27" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="28" t="s">
+      <c r="A52" s="27" t="s">
         <v>142</v>
       </c>
-      <c r="B52" s="28" t="s">
+      <c r="B52" s="27" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="28" t="s">
+      <c r="A53" s="27" t="s">
         <v>144</v>
       </c>
-      <c r="B53" s="28" t="s">
+      <c r="B53" s="27" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="28" t="s">
+      <c r="A54" s="27" t="s">
         <v>146</v>
       </c>
-      <c r="B54" s="28" t="s">
+      <c r="B54" s="27" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="28" t="s">
+      <c r="A55" s="27" t="s">
         <v>148</v>
       </c>
-      <c r="B55" s="28" t="s">
+      <c r="B55" s="27" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="28" t="s">
+      <c r="A56" s="27" t="s">
         <v>150</v>
       </c>
-      <c r="B56" s="28" t="s">
+      <c r="B56" s="27" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="28" t="s">
+      <c r="A57" s="27" t="s">
         <v>152</v>
       </c>
-      <c r="B57" s="28" t="s">
+      <c r="B57" s="27" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="28" t="s">
+      <c r="A58" s="27" t="s">
         <v>154</v>
       </c>
-      <c r="B58" s="28" t="s">
+      <c r="B58" s="27" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="28" t="s">
+      <c r="A59" s="27" t="s">
         <v>156</v>
       </c>
-      <c r="B59" s="28" t="s">
+      <c r="B59" s="27" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="28" t="s">
+      <c r="A60" s="27" t="s">
         <v>158</v>
       </c>
-      <c r="B60" s="28" t="s">
+      <c r="B60" s="27" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="28" t="s">
+      <c r="A61" s="27" t="s">
         <v>160</v>
       </c>
-      <c r="B61" s="28" t="s">
+      <c r="B61" s="27" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="28" t="s">
+      <c r="A62" s="27" t="s">
         <v>162</v>
       </c>
-      <c r="B62" s="28" t="s">
+      <c r="B62" s="27" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="28" t="s">
+      <c r="A63" s="27" t="s">
         <v>164</v>
       </c>
-      <c r="B63" s="28" t="s">
+      <c r="B63" s="27" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="28" t="s">
+      <c r="A64" s="27" t="s">
         <v>166</v>
       </c>
-      <c r="B64" s="28" t="s">
+      <c r="B64" s="27" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="28" t="s">
+      <c r="A65" s="27" t="s">
         <v>168</v>
       </c>
-      <c r="B65" s="28" t="s">
+      <c r="B65" s="27" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="28" t="s">
+      <c r="A66" s="27" t="s">
         <v>170</v>
       </c>
-      <c r="B66" s="28" t="s">
+      <c r="B66" s="27" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A67" s="28" t="s">
+      <c r="A67" s="27" t="s">
         <v>172</v>
       </c>
-      <c r="B67" s="28" t="s">
+      <c r="B67" s="27" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A68" s="28" t="s">
+      <c r="A68" s="27" t="s">
         <v>174</v>
       </c>
-      <c r="B68" s="28" t="s">
+      <c r="B68" s="27" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A69" s="28" t="s">
+      <c r="A69" s="27" t="s">
         <v>176</v>
       </c>
-      <c r="B69" s="28" t="s">
+      <c r="B69" s="27" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A70" s="28" t="s">
+      <c r="A70" s="27" t="s">
         <v>178</v>
       </c>
-      <c r="B70" s="28" t="s">
+      <c r="B70" s="27" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A71" s="28" t="s">
+      <c r="A71" s="27" t="s">
         <v>180</v>
       </c>
-      <c r="B71" s="28" t="s">
+      <c r="B71" s="27" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A72" s="28" t="s">
+      <c r="A72" s="27" t="s">
         <v>182</v>
       </c>
-      <c r="B72" s="28" t="s">
+      <c r="B72" s="27" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A73" s="28" t="s">
+      <c r="A73" s="27" t="s">
         <v>184</v>
       </c>
-      <c r="B73" s="28" t="s">
+      <c r="B73" s="27" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A74" s="28" t="s">
+      <c r="A74" s="27" t="s">
         <v>186</v>
       </c>
-      <c r="B74" s="28" t="s">
+      <c r="B74" s="27" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A75" s="28" t="s">
+      <c r="A75" s="27" t="s">
         <v>188</v>
       </c>
-      <c r="B75" s="28" t="s">
+      <c r="B75" s="27" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A76" s="28" t="s">
+      <c r="A76" s="27" t="s">
         <v>190</v>
       </c>
-      <c r="B76" s="28" t="s">
+      <c r="B76" s="27" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A77" s="28" t="s">
+      <c r="A77" s="27" t="s">
         <v>192</v>
       </c>
-      <c r="B77" s="28" t="s">
+      <c r="B77" s="27" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A78" s="28" t="s">
+      <c r="A78" s="27" t="s">
         <v>194</v>
       </c>
-      <c r="B78" s="28" t="s">
+      <c r="B78" s="27" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A79" s="28" t="s">
+      <c r="A79" s="27" t="s">
         <v>196</v>
       </c>
-      <c r="B79" s="28" t="s">
+      <c r="B79" s="27" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A80" s="28" t="s">
+      <c r="A80" s="27" t="s">
         <v>198</v>
       </c>
-      <c r="B80" s="28" t="s">
+      <c r="B80" s="27" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A81" s="28" t="s">
+      <c r="A81" s="27" t="s">
         <v>200</v>
       </c>
-      <c r="B81" s="28" t="s">
+      <c r="B81" s="27" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A82" s="28" t="s">
+      <c r="A82" s="27" t="s">
         <v>202</v>
       </c>
-      <c r="B82" s="28" t="s">
+      <c r="B82" s="27" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A83" s="28" t="s">
+      <c r="A83" s="27" t="s">
         <v>204</v>
       </c>
-      <c r="B83" s="28" t="s">
+      <c r="B83" s="27" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A84" s="28" t="s">
+      <c r="A84" s="27" t="s">
         <v>206</v>
       </c>
-      <c r="B84" s="28" t="s">
+      <c r="B84" s="27" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A85" s="28" t="s">
+      <c r="A85" s="27" t="s">
         <v>208</v>
       </c>
-      <c r="B85" s="28" t="s">
+      <c r="B85" s="27" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A86" s="28" t="s">
+      <c r="A86" s="27" t="s">
         <v>210</v>
       </c>
-      <c r="B86" s="28" t="s">
+      <c r="B86" s="27" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A87" s="28" t="s">
+      <c r="A87" s="27" t="s">
         <v>212</v>
       </c>
-      <c r="B87" s="28" t="s">
+      <c r="B87" s="27" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A88" s="28" t="s">
+      <c r="A88" s="27" t="s">
         <v>214</v>
       </c>
-      <c r="B88" s="28" t="s">
+      <c r="B88" s="27" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A89" s="28" t="s">
+      <c r="A89" s="27" t="s">
         <v>216</v>
       </c>
-      <c r="B89" s="28" t="s">
+      <c r="B89" s="27" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A90" s="28" t="s">
+      <c r="A90" s="27" t="s">
         <v>218</v>
       </c>
-      <c r="B90" s="28" t="s">
+      <c r="B90" s="27" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A91" s="28" t="s">
+      <c r="A91" s="27" t="s">
         <v>220</v>
       </c>
-      <c r="B91" s="28" t="s">
+      <c r="B91" s="27" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A92" s="28" t="s">
+      <c r="A92" s="27" t="s">
         <v>222</v>
       </c>
-      <c r="B92" s="28" t="s">
+      <c r="B92" s="27" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A93" s="28" t="s">
+      <c r="A93" s="27" t="s">
         <v>224</v>
       </c>
-      <c r="B93" s="28" t="s">
+      <c r="B93" s="27" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A94" s="28" t="s">
+      <c r="A94" s="27" t="s">
         <v>226</v>
       </c>
-      <c r="B94" s="28" t="s">
+      <c r="B94" s="27" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A95" s="28" t="s">
+      <c r="A95" s="27" t="s">
         <v>228</v>
       </c>
-      <c r="B95" s="28" t="s">
+      <c r="B95" s="27" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A96" s="28" t="s">
+      <c r="A96" s="27" t="s">
         <v>230</v>
       </c>
-      <c r="B96" s="28" t="s">
+      <c r="B96" s="27" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A97" s="28" t="s">
+      <c r="A97" s="27" t="s">
         <v>232</v>
       </c>
-      <c r="B97" s="28" t="s">
+      <c r="B97" s="27" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A98" s="28" t="s">
+      <c r="A98" s="27" t="s">
         <v>234</v>
       </c>
-      <c r="B98" s="28" t="s">
+      <c r="B98" s="27" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A99" s="28" t="s">
+      <c r="A99" s="27" t="s">
         <v>236</v>
       </c>
-      <c r="B99" s="28" t="s">
+      <c r="B99" s="27" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A100" s="28" t="s">
+      <c r="A100" s="27" t="s">
         <v>238</v>
       </c>
-      <c r="B100" s="28" t="s">
+      <c r="B100" s="27" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A101" s="28" t="s">
+      <c r="A101" s="27" t="s">
         <v>240</v>
       </c>
-      <c r="B101" s="28" t="s">
+      <c r="B101" s="27" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A102" s="28" t="s">
+      <c r="A102" s="27" t="s">
         <v>242</v>
       </c>
-      <c r="B102" s="28" t="s">
+      <c r="B102" s="27" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A103" s="28" t="s">
+      <c r="A103" s="27" t="s">
         <v>244</v>
       </c>
-      <c r="B103" s="28" t="s">
+      <c r="B103" s="27" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A104" s="28" t="s">
+      <c r="A104" s="27" t="s">
         <v>246</v>
       </c>
-      <c r="B104" s="28" t="s">
+      <c r="B104" s="27" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A105" s="28" t="s">
+      <c r="A105" s="27" t="s">
         <v>248</v>
       </c>
-      <c r="B105" s="28" t="s">
+      <c r="B105" s="27" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A106" s="28" t="s">
+      <c r="A106" s="27" t="s">
         <v>250</v>
       </c>
-      <c r="B106" s="28" t="s">
+      <c r="B106" s="27" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A107" s="28" t="s">
+      <c r="A107" s="27" t="s">
         <v>252</v>
       </c>
-      <c r="B107" s="28" t="s">
+      <c r="B107" s="27" t="s">
         <v>253</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A108" s="28" t="s">
+      <c r="A108" s="27" t="s">
         <v>254</v>
       </c>
-      <c r="B108" s="28" t="s">
+      <c r="B108" s="27" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A109" s="28" t="s">
+      <c r="A109" s="27" t="s">
         <v>256</v>
       </c>
-      <c r="B109" s="28" t="s">
+      <c r="B109" s="27" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A110" s="28" t="s">
+      <c r="A110" s="27" t="s">
         <v>258</v>
       </c>
-      <c r="B110" s="28" t="s">
+      <c r="B110" s="27" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A111" s="28" t="s">
+      <c r="A111" s="27" t="s">
         <v>260</v>
       </c>
-      <c r="B111" s="28" t="s">
+      <c r="B111" s="27" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A112" s="28" t="s">
+      <c r="A112" s="27" t="s">
         <v>262</v>
       </c>
-      <c r="B112" s="28" t="s">
+      <c r="B112" s="27" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A113" s="28" t="s">
+      <c r="A113" s="27" t="s">
         <v>264</v>
       </c>
-      <c r="B113" s="28" t="s">
+      <c r="B113" s="27" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A114" s="28" t="s">
+      <c r="A114" s="27" t="s">
         <v>266</v>
       </c>
-      <c r="B114" s="28" t="s">
+      <c r="B114" s="27" t="s">
         <v>267</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A115" s="28" t="s">
+      <c r="A115" s="27" t="s">
         <v>268</v>
       </c>
-      <c r="B115" s="28" t="s">
+      <c r="B115" s="27" t="s">
         <v>269</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A116" s="28" t="s">
+      <c r="A116" s="27" t="s">
         <v>270</v>
       </c>
-      <c r="B116" s="28" t="s">
+      <c r="B116" s="27" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A117" s="28" t="s">
+      <c r="A117" s="27" t="s">
         <v>272</v>
       </c>
-      <c r="B117" s="28" t="s">
+      <c r="B117" s="27" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="118" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A118" s="28" t="s">
+      <c r="A118" s="27" t="s">
         <v>274</v>
       </c>
-      <c r="B118" s="28" t="s">
+      <c r="B118" s="27" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A119" s="28" t="s">
+      <c r="A119" s="27" t="s">
         <v>276</v>
       </c>
-      <c r="B119" s="28" t="s">
+      <c r="B119" s="27" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="120" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A120" s="28" t="s">
+      <c r="A120" s="27" t="s">
         <v>278</v>
       </c>
-      <c r="B120" s="28" t="s">
+      <c r="B120" s="27" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="121" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A121" s="28" t="s">
+      <c r="A121" s="27" t="s">
         <v>280</v>
       </c>
-      <c r="B121" s="28" t="s">
+      <c r="B121" s="27" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="122" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A122" s="28" t="s">
+      <c r="A122" s="27" t="s">
         <v>282</v>
       </c>
-      <c r="B122" s="28" t="s">
+      <c r="B122" s="27" t="s">
         <v>283</v>
       </c>
     </row>
     <row r="123" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A123" s="28" t="s">
+      <c r="A123" s="27" t="s">
         <v>284</v>
       </c>
-      <c r="B123" s="28" t="s">
+      <c r="B123" s="27" t="s">
         <v>285</v>
       </c>
     </row>
     <row r="124" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A124" s="28" t="s">
+      <c r="A124" s="27" t="s">
         <v>286</v>
       </c>
-      <c r="B124" s="28" t="s">
+      <c r="B124" s="27" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="125" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A125" s="28" t="s">
+      <c r="A125" s="27" t="s">
         <v>288</v>
       </c>
-      <c r="B125" s="28" t="s">
+      <c r="B125" s="27" t="s">
         <v>289</v>
       </c>
     </row>
     <row r="126" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A126" s="28" t="s">
+      <c r="A126" s="27" t="s">
         <v>290</v>
       </c>
-      <c r="B126" s="28" t="s">
+      <c r="B126" s="27" t="s">
         <v>291</v>
       </c>
     </row>
     <row r="127" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A127" s="28" t="s">
+      <c r="A127" s="27" t="s">
         <v>292</v>
       </c>
-      <c r="B127" s="28" t="s">
+      <c r="B127" s="27" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="128" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A128" s="28" t="s">
+      <c r="A128" s="27" t="s">
         <v>294</v>
       </c>
-      <c r="B128" s="28" t="s">
+      <c r="B128" s="27" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="129" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A129" s="28" t="s">
+      <c r="A129" s="27" t="s">
         <v>296</v>
       </c>
-      <c r="B129" s="28" t="s">
+      <c r="B129" s="27" t="s">
         <v>297</v>
       </c>
     </row>
     <row r="130" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A130" s="28" t="s">
+      <c r="A130" s="27" t="s">
         <v>298</v>
       </c>
-      <c r="B130" s="28" t="s">
+      <c r="B130" s="27" t="s">
         <v>299</v>
       </c>
     </row>
     <row r="131" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A131" s="28" t="s">
+      <c r="A131" s="27" t="s">
         <v>300</v>
       </c>
-      <c r="B131" s="28" t="s">
+      <c r="B131" s="27" t="s">
         <v>301</v>
       </c>
     </row>
     <row r="132" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A132" s="28" t="s">
+      <c r="A132" s="27" t="s">
         <v>302</v>
       </c>
-      <c r="B132" s="28" t="s">
+      <c r="B132" s="27" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="133" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A133" s="28" t="s">
+      <c r="A133" s="27" t="s">
         <v>304</v>
       </c>
-      <c r="B133" s="28" t="s">
+      <c r="B133" s="27" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="134" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A134" s="28" t="s">
+      <c r="A134" s="27" t="s">
         <v>306</v>
       </c>
-      <c r="B134" s="28" t="s">
+      <c r="B134" s="27" t="s">
         <v>307</v>
       </c>
     </row>
     <row r="135" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A135" s="28" t="s">
+      <c r="A135" s="27" t="s">
         <v>308</v>
       </c>
-      <c r="B135" s="28" t="s">
+      <c r="B135" s="27" t="s">
         <v>309</v>
       </c>
     </row>
     <row r="136" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A136" s="28" t="s">
+      <c r="A136" s="27" t="s">
         <v>310</v>
       </c>
-      <c r="B136" s="28" t="s">
+      <c r="B136" s="27" t="s">
         <v>311</v>
       </c>
     </row>
     <row r="137" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A137" s="28" t="s">
+      <c r="A137" s="27" t="s">
         <v>312</v>
       </c>
-      <c r="B137" s="28" t="s">
+      <c r="B137" s="27" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="138" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A138" s="28" t="s">
+      <c r="A138" s="27" t="s">
         <v>314</v>
       </c>
-      <c r="B138" s="28" t="s">
+      <c r="B138" s="27" t="s">
         <v>315</v>
       </c>
     </row>
     <row r="139" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A139" s="28" t="s">
+      <c r="A139" s="27" t="s">
         <v>316</v>
       </c>
-      <c r="B139" s="28" t="s">
+      <c r="B139" s="27" t="s">
         <v>317</v>
       </c>
     </row>
     <row r="140" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A140" s="28" t="s">
+      <c r="A140" s="27" t="s">
         <v>318</v>
       </c>
-      <c r="B140" s="28" t="s">
+      <c r="B140" s="27" t="s">
         <v>319</v>
       </c>
     </row>
     <row r="141" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A141" s="28" t="s">
+      <c r="A141" s="27" t="s">
         <v>320</v>
       </c>
-      <c r="B141" s="28" t="s">
+      <c r="B141" s="27" t="s">
         <v>321</v>
       </c>
     </row>
     <row r="142" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A142" s="28" t="s">
+      <c r="A142" s="27" t="s">
         <v>322</v>
       </c>
-      <c r="B142" s="28" t="s">
+      <c r="B142" s="27" t="s">
         <v>323</v>
       </c>
     </row>
     <row r="143" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A143" s="28" t="s">
+      <c r="A143" s="27" t="s">
         <v>324</v>
       </c>
-      <c r="B143" s="28" t="s">
+      <c r="B143" s="27" t="s">
         <v>325</v>
       </c>
     </row>
     <row r="144" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A144" s="28" t="s">
+      <c r="A144" s="27" t="s">
         <v>326</v>
       </c>
-      <c r="B144" s="28" t="s">
+      <c r="B144" s="27" t="s">
         <v>327</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A145" s="28" t="s">
+      <c r="A145" s="27" t="s">
         <v>328</v>
       </c>
-      <c r="B145" s="28" t="s">
+      <c r="B145" s="27" t="s">
         <v>329</v>
       </c>
     </row>
     <row r="146" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A146" s="28" t="s">
+      <c r="A146" s="27" t="s">
         <v>330</v>
       </c>
-      <c r="B146" s="28" t="s">
+      <c r="B146" s="27" t="s">
         <v>331</v>
       </c>
     </row>
     <row r="147" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A147" s="28" t="s">
+      <c r="A147" s="27" t="s">
         <v>332</v>
       </c>
-      <c r="B147" s="28" t="s">
+      <c r="B147" s="27" t="s">
         <v>333</v>
       </c>
     </row>
     <row r="148" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A148" s="28" t="s">
+      <c r="A148" s="27" t="s">
         <v>334</v>
       </c>
-      <c r="B148" s="28" t="s">
+      <c r="B148" s="27" t="s">
         <v>335</v>
       </c>
     </row>
     <row r="149" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A149" s="28" t="s">
+      <c r="A149" s="27" t="s">
         <v>336</v>
       </c>
-      <c r="B149" s="28" t="s">
+      <c r="B149" s="27" t="s">
         <v>337</v>
       </c>
     </row>
     <row r="150" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A150" s="28" t="s">
+      <c r="A150" s="27" t="s">
         <v>338</v>
       </c>
-      <c r="B150" s="28" t="s">
+      <c r="B150" s="27" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="151" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A151" s="28" t="s">
+      <c r="A151" s="27" t="s">
         <v>340</v>
       </c>
-      <c r="B151" s="28" t="s">
+      <c r="B151" s="27" t="s">
         <v>341</v>
       </c>
     </row>
     <row r="152" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A152" s="28" t="s">
+      <c r="A152" s="27" t="s">
         <v>342</v>
       </c>
-      <c r="B152" s="28" t="s">
+      <c r="B152" s="27" t="s">
         <v>343</v>
       </c>
     </row>
     <row r="153" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A153" s="28" t="s">
+      <c r="A153" s="27" t="s">
         <v>344</v>
       </c>
-      <c r="B153" s="28" t="s">
+      <c r="B153" s="27" t="s">
         <v>345</v>
       </c>
     </row>
     <row r="154" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A154" s="28" t="s">
+      <c r="A154" s="27" t="s">
         <v>346</v>
       </c>
-      <c r="B154" s="28" t="s">
+      <c r="B154" s="27" t="s">
         <v>347</v>
       </c>
     </row>
     <row r="155" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A155" s="28" t="s">
+      <c r="A155" s="27" t="s">
         <v>348</v>
       </c>
-      <c r="B155" s="28" t="s">
+      <c r="B155" s="27" t="s">
         <v>349</v>
       </c>
     </row>
     <row r="156" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A156" s="28" t="s">
+      <c r="A156" s="27" t="s">
         <v>350</v>
       </c>
-      <c r="B156" s="28" t="s">
+      <c r="B156" s="27" t="s">
         <v>351</v>
       </c>
     </row>
     <row r="157" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A157" s="28" t="s">
+      <c r="A157" s="27" t="s">
         <v>352</v>
       </c>
-      <c r="B157" s="28" t="s">
+      <c r="B157" s="27" t="s">
         <v>353</v>
       </c>
     </row>
     <row r="158" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A158" s="28" t="s">
+      <c r="A158" s="27" t="s">
         <v>354</v>
       </c>
-      <c r="B158" s="28" t="s">
+      <c r="B158" s="27" t="s">
         <v>355</v>
       </c>
     </row>
     <row r="159" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A159" s="28" t="s">
+      <c r="A159" s="27" t="s">
         <v>356</v>
       </c>
-      <c r="B159" s="28" t="s">
+      <c r="B159" s="27" t="s">
         <v>357</v>
       </c>
     </row>
     <row r="160" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A160" s="28" t="s">
+      <c r="A160" s="27" t="s">
         <v>358</v>
       </c>
-      <c r="B160" s="28" t="s">
+      <c r="B160" s="27" t="s">
         <v>359</v>
       </c>
     </row>
     <row r="161" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A161" s="28" t="s">
+      <c r="A161" s="27" t="s">
         <v>360</v>
       </c>
-      <c r="B161" s="28" t="s">
+      <c r="B161" s="27" t="s">
         <v>361</v>
       </c>
     </row>
     <row r="162" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A162" s="28" t="s">
+      <c r="A162" s="27" t="s">
         <v>362</v>
       </c>
-      <c r="B162" s="28" t="s">
+      <c r="B162" s="27" t="s">
         <v>363</v>
       </c>
     </row>
     <row r="163" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A163" s="28" t="s">
+      <c r="A163" s="27" t="s">
         <v>364</v>
       </c>
-      <c r="B163" s="28" t="s">
+      <c r="B163" s="27" t="s">
         <v>365</v>
       </c>
     </row>
     <row r="164" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A164" s="28" t="s">
+      <c r="A164" s="27" t="s">
         <v>366</v>
       </c>
-      <c r="B164" s="28" t="s">
+      <c r="B164" s="27" t="s">
         <v>367</v>
       </c>
     </row>
     <row r="165" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A165" s="28" t="s">
+      <c r="A165" s="27" t="s">
         <v>368</v>
       </c>
-      <c r="B165" s="28" t="s">
+      <c r="B165" s="27" t="s">
         <v>369</v>
       </c>
     </row>
     <row r="166" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A166" s="28" t="s">
+      <c r="A166" s="27" t="s">
         <v>370</v>
       </c>
-      <c r="B166" s="28" t="s">
+      <c r="B166" s="27" t="s">
         <v>371</v>
       </c>
     </row>
     <row r="167" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A167" s="28" t="s">
+      <c r="A167" s="27" t="s">
         <v>372</v>
       </c>
-      <c r="B167" s="28" t="s">
+      <c r="B167" s="27" t="s">
         <v>373</v>
       </c>
     </row>
     <row r="168" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A168" s="28" t="s">
+      <c r="A168" s="27" t="s">
         <v>374</v>
       </c>
-      <c r="B168" s="28" t="s">
+      <c r="B168" s="27" t="s">
         <v>375</v>
       </c>
     </row>
     <row r="169" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A169" s="28" t="s">
+      <c r="A169" s="27" t="s">
         <v>376</v>
       </c>
-      <c r="B169" s="28" t="s">
+      <c r="B169" s="27" t="s">
         <v>377</v>
       </c>
     </row>
     <row r="170" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A170" s="28" t="s">
+      <c r="A170" s="27" t="s">
         <v>378</v>
       </c>
-      <c r="B170" s="28" t="s">
+      <c r="B170" s="27" t="s">
         <v>379</v>
       </c>
     </row>
     <row r="171" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A171" s="28" t="s">
+      <c r="A171" s="27" t="s">
         <v>380</v>
       </c>
-      <c r="B171" s="28" t="s">
+      <c r="B171" s="27" t="s">
         <v>381</v>
       </c>
     </row>
     <row r="172" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A172" s="28" t="s">
+      <c r="A172" s="27" t="s">
         <v>382</v>
       </c>
-      <c r="B172" s="28" t="s">
+      <c r="B172" s="27" t="s">
         <v>383</v>
       </c>
     </row>
     <row r="173" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A173" s="28" t="s">
+      <c r="A173" s="27" t="s">
         <v>384</v>
       </c>
-      <c r="B173" s="28" t="s">
+      <c r="B173" s="27" t="s">
         <v>385</v>
       </c>
     </row>
     <row r="174" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A174" s="28" t="s">
+      <c r="A174" s="27" t="s">
         <v>386</v>
       </c>
-      <c r="B174" s="28" t="s">
+      <c r="B174" s="27" t="s">
         <v>387</v>
       </c>
     </row>
     <row r="175" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A175" s="28" t="s">
+      <c r="A175" s="27" t="s">
         <v>388</v>
       </c>
-      <c r="B175" s="28" t="s">
+      <c r="B175" s="27" t="s">
         <v>389</v>
       </c>
     </row>
     <row r="176" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A176" s="28" t="s">
+      <c r="A176" s="27" t="s">
         <v>390</v>
       </c>
-      <c r="B176" s="28" t="s">
+      <c r="B176" s="27" t="s">
         <v>391</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A177" s="28" t="s">
+      <c r="A177" s="27" t="s">
         <v>392</v>
       </c>
-      <c r="B177" s="28" t="s">
+      <c r="B177" s="27" t="s">
         <v>393</v>
       </c>
     </row>
     <row r="178" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A178" s="28" t="s">
+      <c r="A178" s="27" t="s">
         <v>394</v>
       </c>
-      <c r="B178" s="28" t="s">
+      <c r="B178" s="27" t="s">
         <v>395</v>
       </c>
     </row>
     <row r="179" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A179" s="28" t="s">
+      <c r="A179" s="27" t="s">
         <v>396</v>
       </c>
-      <c r="B179" s="28" t="s">
+      <c r="B179" s="27" t="s">
         <v>397</v>
       </c>
     </row>
     <row r="180" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A180" s="28" t="s">
+      <c r="A180" s="27" t="s">
         <v>398</v>
       </c>
-      <c r="B180" s="28" t="s">
+      <c r="B180" s="27" t="s">
         <v>399</v>
       </c>
     </row>
     <row r="181" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A181" s="28" t="s">
+      <c r="A181" s="27" t="s">
         <v>400</v>
       </c>
-      <c r="B181" s="28" t="s">
+      <c r="B181" s="27" t="s">
         <v>401</v>
       </c>
     </row>
     <row r="182" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A182" s="28" t="s">
+      <c r="A182" s="27" t="s">
         <v>402</v>
       </c>
-      <c r="B182" s="28" t="s">
+      <c r="B182" s="27" t="s">
         <v>403</v>
       </c>
     </row>
     <row r="183" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A183" s="28" t="s">
+      <c r="A183" s="27" t="s">
         <v>404</v>
       </c>
-      <c r="B183" s="28" t="s">
+      <c r="B183" s="27" t="s">
         <v>405</v>
       </c>
     </row>
     <row r="184" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A184" s="28" t="s">
+      <c r="A184" s="27" t="s">
         <v>406</v>
       </c>
-      <c r="B184" s="28" t="s">
+      <c r="B184" s="27" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="185" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A185" s="28" t="s">
+      <c r="A185" s="27" t="s">
         <v>408</v>
       </c>
-      <c r="B185" s="28" t="s">
+      <c r="B185" s="27" t="s">
         <v>409</v>
       </c>
     </row>
     <row r="186" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A186" s="28" t="s">
+      <c r="A186" s="27" t="s">
         <v>410</v>
       </c>
-      <c r="B186" s="28" t="s">
+      <c r="B186" s="27" t="s">
         <v>411</v>
       </c>
     </row>
     <row r="187" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A187" s="28" t="s">
+      <c r="A187" s="27" t="s">
         <v>412</v>
       </c>
-      <c r="B187" s="28" t="s">
+      <c r="B187" s="27" t="s">
         <v>413</v>
       </c>
     </row>
     <row r="188" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A188" s="28" t="s">
+      <c r="A188" s="27" t="s">
         <v>414</v>
       </c>
-      <c r="B188" s="28" t="s">
+      <c r="B188" s="27" t="s">
         <v>415</v>
       </c>
     </row>
     <row r="189" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A189" s="28" t="s">
+      <c r="A189" s="27" t="s">
         <v>416</v>
       </c>
-      <c r="B189" s="28" t="s">
+      <c r="B189" s="27" t="s">
         <v>417</v>
       </c>
     </row>
     <row r="190" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A190" s="28" t="s">
+      <c r="A190" s="27" t="s">
         <v>418</v>
       </c>
-      <c r="B190" s="28" t="s">
+      <c r="B190" s="27" t="s">
         <v>419</v>
       </c>
     </row>
     <row r="191" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A191" s="28" t="s">
+      <c r="A191" s="27" t="s">
         <v>420</v>
       </c>
-      <c r="B191" s="28" t="s">
+      <c r="B191" s="27" t="s">
         <v>421</v>
       </c>
     </row>
     <row r="192" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A192" s="28" t="s">
+      <c r="A192" s="27" t="s">
         <v>422</v>
       </c>
-      <c r="B192" s="28" t="s">
+      <c r="B192" s="27" t="s">
         <v>423</v>
       </c>
     </row>
     <row r="193" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A193" s="28" t="s">
+      <c r="A193" s="27" t="s">
         <v>424</v>
       </c>
-      <c r="B193" s="28" t="s">
+      <c r="B193" s="27" t="s">
         <v>425</v>
       </c>
     </row>
     <row r="194" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A194" s="28" t="s">
+      <c r="A194" s="27" t="s">
         <v>426</v>
       </c>
-      <c r="B194" s="28" t="s">
+      <c r="B194" s="27" t="s">
         <v>427</v>
       </c>
     </row>
     <row r="195" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A195" s="28" t="s">
+      <c r="A195" s="27" t="s">
         <v>428</v>
       </c>
-      <c r="B195" s="28" t="s">
+      <c r="B195" s="27" t="s">
         <v>429</v>
       </c>
     </row>
     <row r="196" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A196" s="28" t="s">
+      <c r="A196" s="27" t="s">
         <v>430</v>
       </c>
-      <c r="B196" s="28" t="s">
+      <c r="B196" s="27" t="s">
         <v>431</v>
       </c>
     </row>
     <row r="197" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A197" s="28" t="s">
+      <c r="A197" s="27" t="s">
         <v>432</v>
       </c>
-      <c r="B197" s="28" t="s">
+      <c r="B197" s="27" t="s">
         <v>433</v>
       </c>
     </row>
     <row r="198" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A198" s="28" t="s">
+      <c r="A198" s="27" t="s">
         <v>434</v>
       </c>
-      <c r="B198" s="28" t="s">
+      <c r="B198" s="27" t="s">
         <v>435</v>
       </c>
     </row>
     <row r="199" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A199" s="28" t="s">
+      <c r="A199" s="27" t="s">
         <v>436</v>
       </c>
-      <c r="B199" s="28" t="s">
+      <c r="B199" s="27" t="s">
         <v>437</v>
       </c>
     </row>
     <row r="200" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A200" s="28" t="s">
+      <c r="A200" s="27" t="s">
         <v>438</v>
       </c>
-      <c r="B200" s="28" t="s">
+      <c r="B200" s="27" t="s">
         <v>439</v>
       </c>
     </row>
     <row r="201" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A201" s="28" t="s">
+      <c r="A201" s="27" t="s">
         <v>440</v>
       </c>
-      <c r="B201" s="28" t="s">
+      <c r="B201" s="27" t="s">
         <v>441</v>
       </c>
     </row>
     <row r="202" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A202" s="28" t="s">
+      <c r="A202" s="27" t="s">
         <v>442</v>
       </c>
-      <c r="B202" s="28" t="s">
+      <c r="B202" s="27" t="s">
         <v>443</v>
       </c>
     </row>
     <row r="203" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A203" s="28" t="s">
+      <c r="A203" s="27" t="s">
         <v>444</v>
       </c>
-      <c r="B203" s="28" t="s">
+      <c r="B203" s="27" t="s">
         <v>445</v>
       </c>
     </row>
     <row r="204" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A204" s="28" t="s">
+      <c r="A204" s="27" t="s">
         <v>446</v>
       </c>
-      <c r="B204" s="28" t="s">
+      <c r="B204" s="27" t="s">
         <v>447</v>
       </c>
     </row>
     <row r="205" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A205" s="28" t="s">
+      <c r="A205" s="27" t="s">
         <v>448</v>
       </c>
-      <c r="B205" s="28" t="s">
+      <c r="B205" s="27" t="s">
         <v>449</v>
       </c>
     </row>
     <row r="206" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A206" s="28" t="s">
+      <c r="A206" s="27" t="s">
         <v>450</v>
       </c>
-      <c r="B206" s="28" t="s">
+      <c r="B206" s="27" t="s">
         <v>451</v>
       </c>
     </row>
     <row r="207" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A207" s="28" t="s">
+      <c r="A207" s="27" t="s">
         <v>452</v>
       </c>
-      <c r="B207" s="28" t="s">
+      <c r="B207" s="27" t="s">
         <v>453</v>
       </c>
     </row>
     <row r="208" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A208" s="28" t="s">
+      <c r="A208" s="27" t="s">
         <v>454</v>
       </c>
-      <c r="B208" s="28" t="s">
+      <c r="B208" s="27" t="s">
         <v>455</v>
       </c>
     </row>
     <row r="209" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A209" s="28" t="s">
+      <c r="A209" s="27" t="s">
         <v>456</v>
       </c>
-      <c r="B209" s="28" t="s">
+      <c r="B209" s="27" t="s">
         <v>457</v>
       </c>
     </row>
     <row r="210" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A210" s="28" t="s">
+      <c r="A210" s="27" t="s">
         <v>458</v>
       </c>
-      <c r="B210" s="28" t="s">
+      <c r="B210" s="27" t="s">
         <v>459</v>
       </c>
     </row>
     <row r="211" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A211" s="28" t="s">
+      <c r="A211" s="27" t="s">
         <v>460</v>
       </c>
-      <c r="B211" s="28" t="s">
+      <c r="B211" s="27" t="s">
         <v>461</v>
       </c>
     </row>
     <row r="212" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A212" s="28" t="s">
+      <c r="A212" s="27" t="s">
         <v>462</v>
       </c>
-      <c r="B212" s="28" t="s">
+      <c r="B212" s="27" t="s">
         <v>463</v>
       </c>
     </row>
     <row r="213" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A213" s="28" t="s">
+      <c r="A213" s="27" t="s">
         <v>464</v>
       </c>
-      <c r="B213" s="28" t="s">
+      <c r="B213" s="27" t="s">
         <v>465</v>
       </c>
     </row>
     <row r="214" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A214" s="28" t="s">
+      <c r="A214" s="27" t="s">
         <v>466</v>
       </c>
-      <c r="B214" s="28" t="s">
+      <c r="B214" s="27" t="s">
         <v>467</v>
       </c>
     </row>
     <row r="215" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A215" s="28" t="s">
+      <c r="A215" s="27" t="s">
         <v>468</v>
       </c>
-      <c r="B215" s="28" t="s">
+      <c r="B215" s="27" t="s">
         <v>469</v>
       </c>
     </row>
     <row r="216" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A216" s="28" t="s">
+      <c r="A216" s="27" t="s">
         <v>470</v>
       </c>
-      <c r="B216" s="28" t="s">
+      <c r="B216" s="27" t="s">
         <v>471</v>
       </c>
     </row>
     <row r="217" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A217" s="28" t="s">
+      <c r="A217" s="27" t="s">
         <v>472</v>
       </c>
-      <c r="B217" s="28" t="s">
+      <c r="B217" s="27" t="s">
         <v>473</v>
       </c>
     </row>
     <row r="218" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A218" s="28" t="s">
+      <c r="A218" s="27" t="s">
         <v>474</v>
       </c>
-      <c r="B218" s="28" t="s">
+      <c r="B218" s="27" t="s">
         <v>475</v>
       </c>
     </row>
     <row r="219" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A219" s="28" t="s">
+      <c r="A219" s="27" t="s">
         <v>476</v>
       </c>
-      <c r="B219" s="28" t="s">
+      <c r="B219" s="27" t="s">
         <v>477</v>
       </c>
     </row>
     <row r="220" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A220" s="28" t="s">
+      <c r="A220" s="27" t="s">
         <v>478</v>
       </c>
-      <c r="B220" s="28" t="s">
+      <c r="B220" s="27" t="s">
         <v>479</v>
       </c>
     </row>
     <row r="221" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A221" s="28" t="s">
+      <c r="A221" s="27" t="s">
         <v>480</v>
       </c>
-      <c r="B221" s="28" t="s">
+      <c r="B221" s="27" t="s">
         <v>481</v>
       </c>
     </row>
     <row r="222" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A222" s="28" t="s">
+      <c r="A222" s="27" t="s">
         <v>482</v>
       </c>
-      <c r="B222" s="28" t="s">
+      <c r="B222" s="27" t="s">
         <v>483</v>
       </c>
     </row>
     <row r="223" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A223" s="28" t="s">
+      <c r="A223" s="27" t="s">
         <v>484</v>
       </c>
-      <c r="B223" s="28" t="s">
+      <c r="B223" s="27" t="s">
         <v>485</v>
       </c>
     </row>
     <row r="224" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A224" s="28" t="s">
+      <c r="A224" s="27" t="s">
         <v>486</v>
       </c>
-      <c r="B224" s="28" t="s">
+      <c r="B224" s="27" t="s">
         <v>487</v>
       </c>
     </row>
     <row r="225" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A225" s="28" t="s">
+      <c r="A225" s="27" t="s">
         <v>488</v>
       </c>
-      <c r="B225" s="28" t="s">
+      <c r="B225" s="27" t="s">
         <v>489</v>
       </c>
     </row>
     <row r="226" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A226" s="28" t="s">
+      <c r="A226" s="27" t="s">
         <v>490</v>
       </c>
-      <c r="B226" s="28" t="s">
+      <c r="B226" s="27" t="s">
         <v>491</v>
       </c>
     </row>
     <row r="227" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A227" s="28" t="s">
+      <c r="A227" s="27" t="s">
         <v>492</v>
       </c>
-      <c r="B227" s="28" t="s">
+      <c r="B227" s="27" t="s">
         <v>493</v>
       </c>
     </row>
     <row r="228" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A228" s="28" t="s">
+      <c r="A228" s="27" t="s">
         <v>494</v>
       </c>
-      <c r="B228" s="28" t="s">
+      <c r="B228" s="27" t="s">
         <v>495</v>
       </c>
     </row>
     <row r="229" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A229" s="28" t="s">
+      <c r="A229" s="27" t="s">
         <v>496</v>
       </c>
-      <c r="B229" s="28" t="s">
+      <c r="B229" s="27" t="s">
         <v>497</v>
       </c>
     </row>
     <row r="230" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A230" s="28" t="s">
+      <c r="A230" s="27" t="s">
         <v>498</v>
       </c>
-      <c r="B230" s="28" t="s">
+      <c r="B230" s="27" t="s">
         <v>499</v>
       </c>
     </row>
     <row r="231" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A231" s="28" t="s">
+      <c r="A231" s="27" t="s">
         <v>500</v>
       </c>
-      <c r="B231" s="28" t="s">
+      <c r="B231" s="27" t="s">
         <v>501</v>
       </c>
     </row>
     <row r="232" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A232" s="28" t="s">
+      <c r="A232" s="27" t="s">
         <v>502</v>
       </c>
-      <c r="B232" s="28" t="s">
+      <c r="B232" s="27" t="s">
         <v>503</v>
       </c>
     </row>
     <row r="233" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A233" s="28" t="s">
+      <c r="A233" s="27" t="s">
         <v>504</v>
       </c>
-      <c r="B233" s="28" t="s">
+      <c r="B233" s="27" t="s">
         <v>505</v>
       </c>
     </row>
     <row r="234" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A234" s="28" t="s">
+      <c r="A234" s="27" t="s">
         <v>506</v>
       </c>
-      <c r="B234" s="28" t="s">
+      <c r="B234" s="27" t="s">
         <v>507</v>
       </c>
     </row>
     <row r="235" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A235" s="28" t="s">
+      <c r="A235" s="27" t="s">
         <v>508</v>
       </c>
-      <c r="B235" s="28" t="s">
+      <c r="B235" s="27" t="s">
         <v>509</v>
       </c>
     </row>
     <row r="236" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A236" s="28" t="s">
+      <c r="A236" s="27" t="s">
         <v>510</v>
       </c>
-      <c r="B236" s="28" t="s">
+      <c r="B236" s="27" t="s">
         <v>511</v>
       </c>
     </row>
     <row r="237" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A237" s="28" t="s">
+      <c r="A237" s="27" t="s">
         <v>512</v>
       </c>
-      <c r="B237" s="28" t="s">
+      <c r="B237" s="27" t="s">
         <v>513</v>
       </c>
     </row>
     <row r="238" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A238" s="28" t="s">
+      <c r="A238" s="27" t="s">
         <v>514</v>
       </c>
-      <c r="B238" s="28" t="s">
+      <c r="B238" s="27" t="s">
         <v>515</v>
       </c>
     </row>
     <row r="239" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A239" s="28" t="s">
+      <c r="A239" s="27" t="s">
         <v>516</v>
       </c>
-      <c r="B239" s="28" t="s">
+      <c r="B239" s="27" t="s">
         <v>517</v>
       </c>
     </row>
     <row r="240" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A240" s="28" t="s">
+      <c r="A240" s="27" t="s">
         <v>518</v>
       </c>
-      <c r="B240" s="28" t="s">
+      <c r="B240" s="27" t="s">
         <v>519</v>
       </c>
     </row>
     <row r="241" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A241" s="28" t="s">
+      <c r="A241" s="27" t="s">
         <v>520</v>
       </c>
-      <c r="B241" s="28" t="s">
+      <c r="B241" s="27" t="s">
         <v>521</v>
       </c>
     </row>
     <row r="242" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A242" s="28" t="s">
+      <c r="A242" s="27" t="s">
         <v>522</v>
       </c>
-      <c r="B242" s="28" t="s">
+      <c r="B242" s="27" t="s">
         <v>523</v>
       </c>
     </row>
     <row r="243" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A243" s="28" t="s">
+      <c r="A243" s="27" t="s">
         <v>524</v>
       </c>
-      <c r="B243" s="28" t="s">
+      <c r="B243" s="27" t="s">
         <v>525</v>
       </c>
     </row>
     <row r="244" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A244" s="28" t="s">
+      <c r="A244" s="27" t="s">
         <v>526</v>
       </c>
-      <c r="B244" s="28" t="s">
+      <c r="B244" s="27" t="s">
         <v>527</v>
       </c>
     </row>
     <row r="245" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A245" s="28" t="s">
+      <c r="A245" s="27" t="s">
         <v>528</v>
       </c>
-      <c r="B245" s="28" t="s">
+      <c r="B245" s="27" t="s">
         <v>529</v>
       </c>
     </row>
     <row r="246" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A246" s="28" t="s">
+      <c r="A246" s="27" t="s">
         <v>530</v>
       </c>
-      <c r="B246" s="28" t="s">
+      <c r="B246" s="27" t="s">
         <v>531</v>
       </c>
     </row>
     <row r="247" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A247" s="28" t="s">
+      <c r="A247" s="27" t="s">
         <v>532</v>
       </c>
-      <c r="B247" s="28" t="s">
+      <c r="B247" s="27" t="s">
         <v>533</v>
       </c>
     </row>
     <row r="248" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A248" s="28" t="s">
+      <c r="A248" s="27" t="s">
         <v>534</v>
       </c>
-      <c r="B248" s="28" t="s">
+      <c r="B248" s="27" t="s">
         <v>535</v>
       </c>
     </row>
     <row r="249" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A249" s="28" t="s">
+      <c r="A249" s="27" t="s">
         <v>536</v>
       </c>
-      <c r="B249" s="28" t="s">
+      <c r="B249" s="27" t="s">
         <v>537</v>
       </c>
     </row>
     <row r="250" spans="1:2" ht="31" x14ac:dyDescent="0.35">
-      <c r="A250" s="28" t="s">
+      <c r="A250" s="27" t="s">
         <v>538</v>
       </c>
-      <c r="B250" s="28" t="s">
+      <c r="B250" s="27" t="s">
         <v>539</v>
       </c>
     </row>
     <row r="251" spans="1:2" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A251" s="28" t="s">
+      <c r="A251" s="27" t="s">
         <v>540</v>
       </c>
-      <c r="B251" s="28" t="s">
+      <c r="B251" s="27" t="s">
         <v>541</v>
       </c>
     </row>
     <row r="252" spans="1:2" ht="36" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A252" s="28" t="s">
+      <c r="A252" s="27" t="s">
         <v>542</v>
       </c>
-      <c r="B252" s="28" t="s">
+      <c r="B252" s="27" t="s">
         <v>543</v>
       </c>
     </row>
     <row r="253" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A253" s="28" t="s">
+      <c r="A253" s="27" t="s">
         <v>544</v>
       </c>
-      <c r="B253" s="28" t="s">
+      <c r="B253" s="27" t="s">
         <v>545</v>
       </c>
     </row>
     <row r="254" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A254" s="28" t="s">
+      <c r="A254" s="27" t="s">
         <v>546</v>
       </c>
-      <c r="B254" s="28" t="s">
+      <c r="B254" s="27" t="s">
         <v>547</v>
       </c>
     </row>
@@ -7219,6 +7300,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="18390984-f7d9-4502-80ba-82ec344db5fb">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="629dd2dc-abea-47e8-ba88-82202e3ee8ef" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D364DC965387FD4EAF4833DDCF640F91" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c7401bc8bddc44f3d87e6545050f3282">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="18390984-f7d9-4502-80ba-82ec344db5fb" xmlns:ns3="629dd2dc-abea-47e8-ba88-82202e3ee8ef" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fc3cb6a02f8baa81433631181c409fee" ns2:_="" ns3:_="">
     <xsd:import namespace="18390984-f7d9-4502-80ba-82ec344db5fb"/>
@@ -7455,27 +7556,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C2A0AF4-2234-45DE-BCD6-060ACA865D30}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="18390984-f7d9-4502-80ba-82ec344db5fb"/>
+    <ds:schemaRef ds:uri="629dd2dc-abea-47e8-ba88-82202e3ee8ef"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="18390984-f7d9-4502-80ba-82ec344db5fb">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="629dd2dc-abea-47e8-ba88-82202e3ee8ef" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A5056AD-6F82-4433-81E7-2CF7DDF58706}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A6CC910-0FFF-41DD-A80E-A1312D067115}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7492,23 +7592,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A5056AD-6F82-4433-81E7-2CF7DDF58706}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C2A0AF4-2234-45DE-BCD6-060ACA865D30}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="18390984-f7d9-4502-80ba-82ec344db5fb"/>
-    <ds:schemaRef ds:uri="629dd2dc-abea-47e8-ba88-82202e3ee8ef"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>